<commit_message>
changes in validation -Delete
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/DataUser.xlsx
+++ b/src/main/resources/Data/DataUser.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>email</t>
   </si>
@@ -35,6 +35,33 @@
     <t>password</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>endpoint</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>/users/</t>
+  </si>
+  <si>
+    <t>Yei56</t>
+  </si>
+  <si>
+    <t>Yeimy Lorena</t>
+  </si>
+  <si>
     <t>firstname</t>
   </si>
   <si>
@@ -44,71 +71,29 @@
     <t>street</t>
   </si>
   <si>
+    <t>Marin</t>
+  </si>
+  <si>
+    <t>cra 555</t>
+  </si>
+  <si>
+    <t>79 a</t>
+  </si>
+  <si>
     <t>zipcode</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>Nana@gmail.com</t>
-  </si>
-  <si>
-    <t>79 a</t>
-  </si>
-  <si>
-    <t>cra 555</t>
-  </si>
-  <si>
-    <t>11111</t>
-  </si>
-  <si>
-    <t>endpoint</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>/users/</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>1-570-236-7033</t>
-  </si>
-  <si>
-    <t>yeiLore</t>
-  </si>
-  <si>
-    <t>Yei56</t>
-  </si>
-  <si>
-    <t>Yeimy</t>
-  </si>
-  <si>
-    <t>Marin</t>
-  </si>
-  <si>
-    <t>Yeimy Lorena</t>
+    <t>yeilorena@gmail.com</t>
+  </si>
+  <si>
+    <t>yei</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,7 +110,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -133,8 +117,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,12 +141,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="FFE2EFDA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -166,43 +158,26 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -211,42 +186,21 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -257,31 +211,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -568,95 +513,95 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="10.90625" style="6"/>
+    <col min="1" max="1" width="19.26953125" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="M1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="6">
+        <v>4444</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="6">
+        <v>11111</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>19</v>
+      <c r="L2" s="6">
+        <v>200</v>
+      </c>
+      <c r="M2" s="6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to modify features
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/DataUser.xlsx
+++ b/src/main/resources/Data/DataUser.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>email</t>
   </si>
@@ -56,37 +56,52 @@
     <t>/users/</t>
   </si>
   <si>
-    <t>Yei56</t>
-  </si>
-  <si>
-    <t>Yeimy Lorena</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>street</t>
-  </si>
-  <si>
-    <t>Marin</t>
-  </si>
-  <si>
-    <t>cra 555</t>
-  </si>
-  <si>
-    <t>79 a</t>
-  </si>
-  <si>
-    <t>zipcode</t>
-  </si>
-  <si>
-    <t>yeilorena@gmail.com</t>
-  </si>
-  <si>
-    <t>yei</t>
+    <t>emailUpdate</t>
+  </si>
+  <si>
+    <t>usernameUpdate</t>
+  </si>
+  <si>
+    <t>passwordUpdate</t>
+  </si>
+  <si>
+    <t>nameUpdate</t>
+  </si>
+  <si>
+    <t>addressUpdate</t>
+  </si>
+  <si>
+    <t>phoneUpdate</t>
+  </si>
+  <si>
+    <t>yeimy@gmail.com</t>
+  </si>
+  <si>
+    <t>Yei456</t>
+  </si>
+  <si>
+    <t>Yei*76H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeimy Lorena </t>
+  </si>
+  <si>
+    <t>Santander</t>
+  </si>
+  <si>
+    <t>Marina@gmail.com</t>
+  </si>
+  <si>
+    <t>Mari369</t>
+  </si>
+  <si>
+    <t>Mar_3$</t>
+  </si>
+  <si>
+    <t>Luz Marina Sosa</t>
+  </si>
+  <si>
+    <t>Sucre/Sder</t>
   </si>
 </sst>
 </file>
@@ -132,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -227,6 +248,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -510,19 +537,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.26953125" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="10.90625" style="2"/>
+    <col min="2" max="9" width="10.90625" style="2"/>
+    <col min="10" max="10" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -533,82 +567,95 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="M1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="N1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="O1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
+      <c r="F2" s="6">
+        <v>3134777820</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H2" s="6">
-        <v>4444</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6">
-        <v>11111</v>
+        <v>200</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="6">
-        <v>200</v>
-      </c>
-      <c r="M2" s="6">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="6">
+        <v>321654987</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>